<commit_message>
Updated Week 1 schedule
</commit_message>
<xml_diff>
--- a/2020/Pennsauken handicaps 2020.xlsx
+++ b/2020/Pennsauken handicaps 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/websites/cscgolf/2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0099271D-ACF5-5A43-AA8C-3700CDB12B10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C180407-C614-AE4E-9736-E1D86740756D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4100" yWindow="2860" windowWidth="22140" windowHeight="12620" tabRatio="214" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>Course</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>x.x</t>
+  </si>
+  <si>
+    <t>Jim Kulcyk</t>
+  </si>
+  <si>
+    <t>Paul Hessler</t>
   </si>
 </sst>
 </file>
@@ -553,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:M23"/>
+  <dimension ref="A3:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="G24" sqref="G24:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -841,7 +847,7 @@
         <v>6.2</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" ref="G21:G22" si="4">ROUND( (B21*$C$16)/113,0)</f>
+        <f t="shared" ref="G21:G25" si="4">ROUND( (B21*$C$16)/113,0)</f>
         <v>7</v>
       </c>
     </row>
@@ -863,6 +869,30 @@
       </c>
       <c r="B23" s="2" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="2">
+        <v>6</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="2">
+        <v>5</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>